<commit_message>
Change to agriculture form
</commit_message>
<xml_diff>
--- a/app/tables/agriculture/forms/agriculture/agriculture.xlsx
+++ b/app/tables/agriculture/forms/agriculture/agriculture.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3540" yWindow="1480" windowWidth="35040" windowHeight="20420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -417,6 +417,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -503,7 +509,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -533,6 +539,9 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
@@ -550,6 +559,9 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -884,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1071,9 +1083,6 @@
       <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="C7" s="5"/>
       <c r="D7" s="12"/>
       <c r="E7" s="5"/>
@@ -1090,7 +1099,6 @@
     </row>
     <row r="8" spans="1:15" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="1" t="s">
         <v>78</v>
@@ -1113,30 +1121,22 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1">
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>80</v>
-      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5" t="b">
-        <v>1</v>
-      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="6"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
@@ -1144,24 +1144,26 @@
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
-        <v>19</v>
+      <c r="D10" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="5" t="b">
-        <v>0</v>
-      </c>
+      <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="J10" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-      <c r="M10" s="6"/>
+      <c r="M10" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
@@ -1170,10 +1172,10 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>60</v>
@@ -1192,15 +1194,21 @@
     </row>
     <row r="12" spans="1:15" s="1" customFormat="1">
       <c r="A12" s="5"/>
-      <c r="B12" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="H12" s="5" t="b">
+        <v>0</v>
+      </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -1209,114 +1217,114 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15" s="1" customFormat="1" ht="30">
+    <row r="13" spans="1:15" s="1" customFormat="1">
       <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="M13" s="5" t="b">
-        <v>1</v>
-      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="6"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15" s="1" customFormat="1" ht="29" customHeight="1">
+    <row r="14" spans="1:15" s="1" customFormat="1" ht="30">
       <c r="A14" s="5"/>
-      <c r="B14" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="6"/>
+      <c r="I14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:15" s="1" customFormat="1" ht="39" customHeight="1">
+    <row r="15" spans="1:15" s="1" customFormat="1" ht="29" customHeight="1">
       <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="B15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" ht="24" customHeight="1">
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" s="1" customFormat="1" ht="39" customHeight="1">
       <c r="A16" s="5"/>
-      <c r="B16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
+      <c r="J16" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="L16" s="5"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="29" customHeight="1">
+      <c r="N16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="24" customHeight="1">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1330,10 +1338,10 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="1:15" s="1" customFormat="1">
+    <row r="18" spans="1:15" s="1" customFormat="1" ht="29" customHeight="1">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1352,7 +1360,7 @@
     <row r="19" spans="1:15" s="1" customFormat="1">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1371,7 +1379,7 @@
     <row r="20" spans="1:15" s="1" customFormat="1">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1387,15 +1395,34 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="1:15" s="8" customFormat="1">
+    <row r="21" spans="1:15" s="1" customFormat="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
-      <c r="M21" s="10"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="1:15" s="8" customFormat="1">
+      <c r="D22" s="5"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
+      <c r="M22" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1413,7 +1440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>